<commit_message>
Alle Testmethoden von Umlauten befreit.
</commit_message>
<xml_diff>
--- a/src/test/testdaten_insert_mitarbeiter/Mitarbeiter.xlsx
+++ b/src/test/testdaten_insert_mitarbeiter/Mitarbeiter.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\test\testdaten_insert_mitarbeiter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEF1736-AF5B-432E-A1DC-DE3DC65DF569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EA755C-8C5E-4007-B790-EF0A07C20DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,9 +70,6 @@
     <t>Strasse</t>
   </si>
   <si>
-    <t>Musterstraße</t>
-  </si>
-  <si>
     <t>Hausnummer</t>
   </si>
   <si>
@@ -281,6 +278,9 @@
   </si>
   <si>
     <t>M100002</t>
+  </si>
+  <si>
+    <t>Musterstrasse</t>
   </si>
 </sst>
 </file>
@@ -789,7 +789,7 @@
   <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -808,10 +808,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -819,7 +819,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -833,23 +833,23 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -878,7 +878,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>12</v>
@@ -886,7 +886,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>5</v>
@@ -894,26 +894,26 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -921,12 +921,12 @@
         <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
@@ -934,7 +934,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="2">
         <v>12358</v>
@@ -942,55 +942,55 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="2">
         <v>1</v>
@@ -998,7 +998,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="4">
         <v>35</v>
@@ -1006,111 +1006,111 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" s="10">
         <v>1</v>
@@ -1118,23 +1118,23 @@
     </row>
     <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="4">
         <v>0</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B44" s="4">
         <v>0</v>
@@ -1150,34 +1150,34 @@
     </row>
     <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1250,58 +1250,58 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1310,7 +1310,7 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>